<commit_message>
Fine name and invoice number changes added
</commit_message>
<xml_diff>
--- a/Process_PO_NonPO_Invoices/Data/Config.xlsx
+++ b/Process_PO_NonPO_Invoices/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpa.uat\Documents\UiPath\SH-Cogent\Process_PO_NonPO_Invoices\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C79040-B13C-43EE-96D7-E029BE4356E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816BD86F-44B9-4DE4-90D5-1EE3D194D9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="174">
   <si>
     <t>Name</t>
   </si>
@@ -447,9 +447,6 @@
     <t>ExcpMsg_NoDocNo</t>
   </si>
   <si>
-    <t>Failed to generate document number. Please check screenshot for more details</t>
-  </si>
-  <si>
     <t>C:\Users\rpa.uat\Documents\XML Archival</t>
   </si>
   <si>
@@ -520,6 +517,39 @@
   </si>
   <si>
     <t>ErpAck folder missing from SFTP</t>
+  </si>
+  <si>
+    <t>ExcpMsgSAPValueEmpty</t>
+  </si>
+  <si>
+    <t>Quantity, Amount or cost centre value is empty in SAP</t>
+  </si>
+  <si>
+    <t>SFTP_Cred_Dev</t>
+  </si>
+  <si>
+    <t>SFTP_Cred_QA</t>
+  </si>
+  <si>
+    <t>Failed to generate document number and no error found under messages. Please check screenshot for more details</t>
+  </si>
+  <si>
+    <t>ExcpMsg_LineitemCountMismatch</t>
+  </si>
+  <si>
+    <t>Line item count from XML &amp; SAP does not match. Please process this invoice manually</t>
+  </si>
+  <si>
+    <t>ExcpMsg_MandatoryValuemising</t>
+  </si>
+  <si>
+    <t>Mandatory value missing in XML file.</t>
+  </si>
+  <si>
+    <t>tag_InvoiceNum</t>
+  </si>
+  <si>
+    <t>InvoiceNumber</t>
   </si>
 </sst>
 </file>
@@ -904,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -987,7 +1017,10 @@
         <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>166</v>
+      </c>
+      <c r="C6" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1074,7 +1107,7 @@
         <v>87</v>
       </c>
       <c r="B15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
@@ -1082,7 +1115,7 @@
         <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
@@ -2097,10 +2130,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:B34"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2283,270 +2316,291 @@
         <v>138</v>
       </c>
       <c r="B17" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18" t="s">
         <v>144</v>
-      </c>
-      <c r="B18" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
+        <v>161</v>
+      </c>
+      <c r="B19" t="s">
         <v>162</v>
       </c>
-      <c r="B19" t="s">
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
+      <c r="B20" t="s">
+        <v>164</v>
+      </c>
+    </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="C21" t="s">
-        <v>38</v>
+        <v>168</v>
+      </c>
+      <c r="B21" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
+        <v>170</v>
+      </c>
+      <c r="B22" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
         <v>36</v>
       </c>
-      <c r="B22">
+      <c r="B25">
         <v>2</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:3" ht="45">
-      <c r="A24" t="s">
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="45">
+      <c r="A27" t="s">
         <v>40</v>
       </c>
-      <c r="B24" t="b">
+      <c r="B27" t="b">
         <v>0</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A26" t="s">
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
         <v>50</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B29" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A27" t="s">
+    <row r="30" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
         <v>126</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B30" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A28" t="s">
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
         <v>130</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B31" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="33" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="34" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" t="s">
+        <v>75</v>
+      </c>
+    </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B35" t="s">
-        <v>74</v>
-      </c>
-      <c r="C35" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B37" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B38" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B40" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" t="s">
-        <v>59</v>
+        <v>96</v>
       </c>
       <c r="B41" t="s">
-        <v>58</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
       <c r="A42" t="s">
-        <v>61</v>
-      </c>
-      <c r="B42" t="s">
-        <v>60</v>
+        <v>98</v>
+      </c>
+      <c r="B42">
+        <v>3000</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="A43" t="s">
-        <v>96</v>
-      </c>
-      <c r="B43" t="s">
-        <v>97</v>
+        <v>99</v>
+      </c>
+      <c r="B43">
+        <v>10000</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1">
       <c r="A44" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B44">
-        <v>5000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1">
       <c r="A45" t="s">
-        <v>99</v>
-      </c>
-      <c r="B45">
-        <v>10000</v>
+        <v>122</v>
+      </c>
+      <c r="B45" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1">
       <c r="A46" t="s">
-        <v>100</v>
-      </c>
-      <c r="B46">
-        <v>20000</v>
+        <v>140</v>
+      </c>
+      <c r="B46" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1">
       <c r="A47" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="B47" t="s">
-        <v>123</v>
+        <v>150</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1">
       <c r="A48" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="B48" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="14.25" customHeight="1">
       <c r="A49" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B49" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="14.25" customHeight="1">
       <c r="A50" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B50" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="14.25" customHeight="1">
       <c r="A51" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="B51" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="14.25" customHeight="1">
       <c r="A52" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="B52" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="14.25" customHeight="1">
       <c r="A53" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B53" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="14.25" customHeight="1">
       <c r="A54" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="B54" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A55" t="s">
-        <v>156</v>
-      </c>
-      <c r="B55" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A56" t="s">
         <v>160</v>
       </c>
-      <c r="B56" t="s">
-        <v>161</v>
-      </c>
-    </row>
+    </row>
+    <row r="55" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="56" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="57" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="58" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="59" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3487,8 +3541,6 @@
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3497,10 +3549,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34508257-0785-4DC0-B956-BF0EF6F76F65}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3521,43 +3573,52 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" ht="18.75">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>172</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
         <v>70</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes to Line item extraction , Changes to system exception, delete file from local folder
</commit_message>
<xml_diff>
--- a/Process_PO_NonPO_Invoices/Data/Config.xlsx
+++ b/Process_PO_NonPO_Invoices/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpa.uat\Documents\UiPath\SH-Cogent\Process_PO_NonPO_Invoices\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpa.uat\Documents\UiPath\Process_PO_NonPO_Invoices\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05343833-A654-47C2-A883-02874AD924E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49C6270-FF2B-4404-9BE5-0A1C3D6F018B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -2138,8 +2138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>